<commit_message>
Added filter staing customer by status
</commit_message>
<xml_diff>
--- a/docs/sample_data.xlsx
+++ b/docs/sample_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="84">
   <si>
     <t>序号</t>
   </si>
@@ -71,7 +71,7 @@
     <t>第一期</t>
   </si>
   <si>
-    <t>2022.4.14</t>
+    <t>2022.4.10</t>
   </si>
   <si>
     <t>住建局</t>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>胡家俊</t>
-  </si>
-  <si>
-    <t>2022.4.10</t>
   </si>
   <si>
     <t>N1叉车</t>
@@ -1494,7 +1491,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1600,7 +1597,7 @@
         <v>12.31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>15</v>
@@ -1618,7 +1615,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K3" s="5">
         <v>18190553888</v>
@@ -1641,16 +1638,16 @@
         <v>1.9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>18</v>
@@ -1665,10 +1662,10 @@
         <v>13890389081</v>
       </c>
       <c r="L4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" ht="123" spans="1:13">
@@ -1682,16 +1679,16 @@
         <v>1.9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>18</v>
@@ -1706,7 +1703,7 @@
         <v>15775150189</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>22</v>
@@ -1723,16 +1720,16 @@
         <v>1.14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>18</v>
@@ -1747,7 +1744,7 @@
         <v>13882023356</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>22</v>
@@ -1764,16 +1761,16 @@
         <v>1.17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>18</v>
@@ -1788,7 +1785,7 @@
         <v>13980260510</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>22</v>
@@ -1805,16 +1802,16 @@
         <v>1.2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>18</v>
@@ -1829,10 +1826,10 @@
         <v>13808166719</v>
       </c>
       <c r="L8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" ht="82" spans="1:13">
@@ -1846,16 +1843,16 @@
         <v>2.6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>18</v>
@@ -1870,10 +1867,10 @@
         <v>17765476062</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" ht="102" spans="1:13">
@@ -1887,34 +1884,34 @@
         <v>2.6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K10" s="5">
         <v>18181524097</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" ht="143" spans="1:13">
@@ -1928,19 +1925,19 @@
         <v>2.6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H11" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>19</v>
@@ -1952,10 +1949,10 @@
         <v>13990628371</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" ht="143" spans="1:13">
@@ -1969,16 +1966,16 @@
         <v>2.7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>18</v>
@@ -1993,10 +1990,10 @@
         <v>15828840500</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" ht="164" spans="1:13">
@@ -2010,16 +2007,16 @@
         <v>2.7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>18</v>
@@ -2034,10 +2031,10 @@
         <v>13079127912</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" ht="123" spans="1:13">
@@ -2051,16 +2048,16 @@
         <v>2.7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>18</v>
@@ -2075,10 +2072,10 @@
         <v>15881979454</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" ht="164" spans="1:13">
@@ -2092,16 +2089,16 @@
         <v>2.7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>18</v>
@@ -2116,10 +2113,10 @@
         <v>18113548598</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" ht="143" spans="1:13">
@@ -2133,16 +2130,16 @@
         <v>2.7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>18</v>
@@ -2157,10 +2154,10 @@
         <v>18160066201</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" ht="123" spans="1:13">
@@ -2174,34 +2171,34 @@
         <v>2.7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="I17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="K17" s="5">
         <v>18183370882</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" ht="123" spans="1:13">
@@ -2215,16 +2212,16 @@
         <v>2.7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>18</v>
@@ -2233,16 +2230,16 @@
         <v>19</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K18" s="5">
         <v>15351308809</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" ht="102" spans="1:13">
@@ -2256,34 +2253,34 @@
         <v>2.8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="H19" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K19" s="5">
         <v>15750632377</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" ht="102" spans="1:13">
@@ -2297,34 +2294,34 @@
         <v>2.8</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="H20" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K20" s="5">
         <v>15750632377</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" ht="82" spans="1:13">
@@ -2338,31 +2335,31 @@
         <v>2.5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="H21" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K21" s="5">
         <v>13881280749</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>22</v>
@@ -2379,31 +2376,31 @@
         <v>1.28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="H22" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K22" s="5">
         <v>13881280749</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
highted changed fields for UPDATE status customer
</commit_message>
<xml_diff>
--- a/docs/sample_data.xlsx
+++ b/docs/sample_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="99">
   <si>
     <t>序号</t>
   </si>
@@ -101,12 +101,18 @@
     <t>N1叉车</t>
   </si>
   <si>
+    <t>181905538881</t>
+  </si>
+  <si>
     <t>徐世清</t>
   </si>
   <si>
     <t>511122197001114736</t>
   </si>
   <si>
+    <t>138903890811</t>
+  </si>
+  <si>
     <t>四川省眉山市东坡区悦兴镇奋勇街2号</t>
   </si>
   <si>
@@ -119,6 +125,9 @@
     <t>511023196810012031</t>
   </si>
   <si>
+    <t>157751501891</t>
+  </si>
+  <si>
     <t>四川省资阳市安岳县长河源乡青石村1组</t>
   </si>
   <si>
@@ -137,6 +146,9 @@
     <t>511181197404214811</t>
   </si>
   <si>
+    <t>139802605101</t>
+  </si>
+  <si>
     <t>四川省乐山市市中区杨湾乡灵官村1组24号</t>
   </si>
   <si>
@@ -146,6 +158,9 @@
     <t>513823200306180014</t>
   </si>
   <si>
+    <t>138081667191</t>
+  </si>
+  <si>
     <t>四川省眉山市彭山区观音镇观音村9组</t>
   </si>
   <si>
@@ -170,6 +185,9 @@
     <t>中专</t>
   </si>
   <si>
+    <t>181815240971</t>
+  </si>
+  <si>
     <t>四川省峨眉山市绥山镇安川村7组</t>
   </si>
   <si>
@@ -179,6 +197,9 @@
     <t>51111219981228353X</t>
   </si>
   <si>
+    <t>139906283711</t>
+  </si>
+  <si>
     <t>四川省乐山市五通桥区牛华镇沔坝村4组169号</t>
   </si>
   <si>
@@ -188,6 +209,9 @@
     <t>511021199010036239</t>
   </si>
   <si>
+    <t>158288405001</t>
+  </si>
+  <si>
     <t>四川省内江市东兴区高梁镇新牌坊村5组15号</t>
   </si>
   <si>
@@ -197,6 +221,9 @@
     <t>510504198710090610</t>
   </si>
   <si>
+    <t>130791279121</t>
+  </si>
+  <si>
     <t>四川省泸州市龙马潭区石洞镇张家祠南路999附1409号</t>
   </si>
   <si>
@@ -215,6 +242,9 @@
     <t>510504198606160658</t>
   </si>
   <si>
+    <t>181135485981</t>
+  </si>
+  <si>
     <t>四川省泸州市龙马潭区石洞镇张家祠南路999附1014号</t>
   </si>
   <si>
@@ -239,6 +269,9 @@
     <t>Q1指挥</t>
   </si>
   <si>
+    <t>181833708821</t>
+  </si>
+  <si>
     <t>四川省乐山市市中区剑峰乡联合村7组176号</t>
   </si>
   <si>
@@ -251,6 +284,9 @@
     <t>51110219710209381X</t>
   </si>
   <si>
+    <t>153513088091</t>
+  </si>
+  <si>
     <t>谭如冰</t>
   </si>
   <si>
@@ -260,6 +296,9 @@
     <t>高中</t>
   </si>
   <si>
+    <t>157506323771</t>
+  </si>
+  <si>
     <t>四川省武胜县龙女镇幸福村3组18号</t>
   </si>
   <si>
@@ -275,10 +314,16 @@
     <t>Q2门式</t>
   </si>
   <si>
+    <t>138812807491</t>
+  </si>
+  <si>
     <t>四川省三台县潼川镇广化橙园村十组007号</t>
   </si>
   <si>
     <t>A特种设备安全管理</t>
+  </si>
+  <si>
+    <t>138812807149</t>
   </si>
 </sst>
 </file>
@@ -961,6 +1006,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1490,8 +1538,8 @@
   <sheetPr/>
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1617,8 +1665,8 @@
       <c r="J3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="5">
-        <v>18190553888</v>
+      <c r="K3" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>21</v>
@@ -1627,7 +1675,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" ht="123" spans="1:13">
+    <row r="4" ht="62" spans="1:13">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1644,10 +1692,10 @@
         <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>18</v>
@@ -1658,17 +1706,17 @@
       <c r="J4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="5">
-        <v>13890389081</v>
+      <c r="K4" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="5" ht="123" spans="1:13">
+    <row r="5" ht="62" spans="1:13">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1685,10 +1733,10 @@
         <v>15</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>18</v>
@@ -1699,11 +1747,11 @@
       <c r="J5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="5">
-        <v>15775150189</v>
+      <c r="K5" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>22</v>
@@ -1726,10 +1774,10 @@
         <v>15</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>18</v>
@@ -1744,13 +1792,13 @@
         <v>13882023356</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" ht="123" spans="1:13">
+    <row r="7" ht="82" spans="1:13">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1767,10 +1815,10 @@
         <v>15</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>18</v>
@@ -1781,17 +1829,17 @@
       <c r="J7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="5">
-        <v>13980260510</v>
+      <c r="K7" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" ht="123" spans="1:13">
+    <row r="8" ht="62" spans="1:13">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1808,10 +1856,10 @@
         <v>15</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>18</v>
@@ -1822,14 +1870,14 @@
       <c r="J8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="5">
-        <v>13808166719</v>
+      <c r="K8" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" ht="82" spans="1:13">
@@ -1849,10 +1897,10 @@
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>18</v>
@@ -1867,13 +1915,13 @@
         <v>17765476062</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="10" ht="102" spans="1:13">
+    <row r="10" ht="62" spans="1:13">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1890,13 +1938,13 @@
         <v>15</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>19</v>
@@ -1904,17 +1952,17 @@
       <c r="J10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="5">
-        <v>18181524097</v>
+      <c r="K10" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="11" ht="143" spans="1:13">
+    <row r="11" ht="82" spans="1:13">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1931,13 +1979,13 @@
         <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>19</v>
@@ -1945,17 +1993,17 @@
       <c r="J11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="5">
-        <v>13990628371</v>
+      <c r="K11" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="12" ht="143" spans="1:13">
+    <row r="12" ht="82" spans="1:13">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1972,10 +2020,10 @@
         <v>15</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>18</v>
@@ -1986,17 +2034,17 @@
       <c r="J12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="5">
-        <v>15828840500</v>
+      <c r="K12" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="13" ht="164" spans="1:13">
+    <row r="13" ht="82" spans="1:13">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -2013,10 +2061,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>18</v>
@@ -2027,14 +2075,14 @@
       <c r="J13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="5">
-        <v>13079127912</v>
+      <c r="K13" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" ht="123" spans="1:13">
@@ -2054,10 +2102,10 @@
         <v>15</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>18</v>
@@ -2072,13 +2120,13 @@
         <v>15881979454</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="15" ht="164" spans="1:13">
+    <row r="15" ht="82" spans="1:13">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -2095,10 +2143,10 @@
         <v>15</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>18</v>
@@ -2109,14 +2157,14 @@
       <c r="J15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="5">
-        <v>18113548598</v>
+      <c r="K15" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" ht="143" spans="1:13">
@@ -2136,10 +2184,10 @@
         <v>15</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>18</v>
@@ -2154,13 +2202,13 @@
         <v>18160066201</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="17" ht="123" spans="1:13">
+    <row r="17" ht="82" spans="1:13">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -2177,31 +2225,31 @@
         <v>15</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K17" s="5">
-        <v>18183370882</v>
+        <v>79</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="18" ht="123" spans="1:13">
+    <row r="18" ht="82" spans="1:13">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -2212,16 +2260,16 @@
         <v>2.7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>18</v>
@@ -2230,19 +2278,19 @@
         <v>19</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K18" s="5">
-        <v>15351308809</v>
+        <v>79</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="19" ht="102" spans="1:13">
+    <row r="19" ht="62" spans="1:13">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -2259,31 +2307,31 @@
         <v>15</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K19" s="5">
-        <v>15750632377</v>
+        <v>79</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="20" ht="102" spans="1:13">
+    <row r="20" ht="62" spans="1:13">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -2300,28 +2348,28 @@
         <v>15</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K20" s="5">
-        <v>15750632377</v>
+        <v>91</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" ht="82" spans="1:13">
@@ -2341,25 +2389,25 @@
         <v>15</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="K21" s="5">
-        <v>13881280749</v>
+        <v>94</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>22</v>
@@ -2382,25 +2430,25 @@
         <v>15</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K22" s="5">
-        <v>13881280749</v>
+        <v>97</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
adjusted data import logic for invalid items
</commit_message>
<xml_diff>
--- a/docs/sample_data.xlsx
+++ b/docs/sample_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="100">
   <si>
     <t>序号</t>
   </si>
@@ -89,25 +89,28 @@
     <t>男</t>
   </si>
   <si>
+    <t>Q2流动式1</t>
+  </si>
+  <si>
+    <t>四川省筠连县双腾镇两河村3组26号</t>
+  </si>
+  <si>
+    <t>胡家俊</t>
+  </si>
+  <si>
+    <t>N1叉车</t>
+  </si>
+  <si>
+    <t>181905538881</t>
+  </si>
+  <si>
+    <t>徐世清</t>
+  </si>
+  <si>
+    <t>511122197001114736</t>
+  </si>
+  <si>
     <t>Q2流动式</t>
-  </si>
-  <si>
-    <t>四川省筠连县双腾镇两河村3组26号</t>
-  </si>
-  <si>
-    <t>胡家俊</t>
-  </si>
-  <si>
-    <t>N1叉车</t>
-  </si>
-  <si>
-    <t>181905538881</t>
-  </si>
-  <si>
-    <t>徐世清</t>
-  </si>
-  <si>
-    <t>511122197001114736</t>
   </si>
   <si>
     <t>138903890811</t>
@@ -1538,8 +1541,8 @@
   <sheetPr/>
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1704,16 +1707,16 @@
         <v>19</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" ht="62" spans="1:13">
@@ -1733,10 +1736,10 @@
         <v>15</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>18</v>
@@ -1745,13 +1748,13 @@
         <v>19</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>22</v>
@@ -1774,10 +1777,10 @@
         <v>15</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>18</v>
@@ -1786,13 +1789,13 @@
         <v>19</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K6" s="5">
         <v>13882023356</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>22</v>
@@ -1815,10 +1818,10 @@
         <v>15</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>18</v>
@@ -1827,13 +1830,13 @@
         <v>19</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>22</v>
@@ -1856,10 +1859,10 @@
         <v>15</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>18</v>
@@ -1868,16 +1871,16 @@
         <v>19</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" ht="82" spans="1:13">
@@ -1897,10 +1900,10 @@
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>18</v>
@@ -1909,16 +1912,16 @@
         <v>19</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K9" s="5">
         <v>17765476062</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" ht="62" spans="1:13">
@@ -1938,13 +1941,13 @@
         <v>15</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>19</v>
@@ -1953,13 +1956,13 @@
         <v>23</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" ht="82" spans="1:13">
@@ -1979,28 +1982,28 @@
         <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" ht="82" spans="1:13">
@@ -2020,10 +2023,10 @@
         <v>15</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>18</v>
@@ -2032,16 +2035,16 @@
         <v>19</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" ht="82" spans="1:13">
@@ -2061,10 +2064,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>18</v>
@@ -2073,16 +2076,16 @@
         <v>19</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" ht="123" spans="1:13">
@@ -2102,10 +2105,10 @@
         <v>15</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>18</v>
@@ -2114,16 +2117,16 @@
         <v>19</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K14" s="5">
         <v>15881979454</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" ht="82" spans="1:13">
@@ -2143,10 +2146,10 @@
         <v>15</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>18</v>
@@ -2155,16 +2158,16 @@
         <v>19</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" ht="143" spans="1:13">
@@ -2184,10 +2187,10 @@
         <v>15</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>18</v>
@@ -2196,16 +2199,16 @@
         <v>19</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K16" s="5">
         <v>18160066201</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" ht="82" spans="1:13">
@@ -2225,28 +2228,28 @@
         <v>15</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" ht="82" spans="1:13">
@@ -2260,16 +2263,16 @@
         <v>2.7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>18</v>
@@ -2278,16 +2281,16 @@
         <v>19</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" ht="62" spans="1:13">
@@ -2307,28 +2310,28 @@
         <v>15</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" ht="62" spans="1:13">
@@ -2348,28 +2351,28 @@
         <v>15</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K20" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="M20" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" ht="82" spans="1:13">
@@ -2389,25 +2392,25 @@
         <v>15</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>22</v>
@@ -2430,25 +2433,25 @@
         <v>15</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J22" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="L22" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Fix ESLint error: replace 'any' type with 'unknown'
Fixed TypeScript linting error in catch block by using 'unknown' type
and proper type guards for error handling.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/sample_data.xlsx
+++ b/docs/sample_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="103">
   <si>
     <t>序号</t>
   </si>
@@ -98,12 +98,18 @@
     <t>胡家俊</t>
   </si>
   <si>
+    <t>住建局1</t>
+  </si>
+  <si>
     <t>N1叉车</t>
   </si>
   <si>
     <t>181905538881</t>
   </si>
   <si>
+    <t>2022.4.10年</t>
+  </si>
+  <si>
     <t>徐世清</t>
   </si>
   <si>
@@ -132,6 +138,9 @@
   </si>
   <si>
     <t>四川省资阳市安岳县长河源乡青石村1组</t>
+  </si>
+  <si>
+    <t>12022.4.10</t>
   </si>
   <si>
     <t>付世华</t>
@@ -1542,7 +1551,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1651,7 +1660,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>16</v>
@@ -1666,10 +1675,10 @@
         <v>19</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>21</v>
@@ -1689,16 +1698,16 @@
         <v>1.9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>18</v>
@@ -1707,16 +1716,16 @@
         <v>19</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" ht="62" spans="1:13">
@@ -1736,10 +1745,10 @@
         <v>15</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>18</v>
@@ -1748,13 +1757,13 @@
         <v>19</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>22</v>
@@ -1771,16 +1780,16 @@
         <v>1.14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>18</v>
@@ -1789,13 +1798,13 @@
         <v>19</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K6" s="5">
         <v>13882023356</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>22</v>
@@ -1818,10 +1827,10 @@
         <v>15</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>18</v>
@@ -1830,13 +1839,13 @@
         <v>19</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>22</v>
@@ -1859,10 +1868,10 @@
         <v>15</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>18</v>
@@ -1871,16 +1880,16 @@
         <v>19</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" ht="82" spans="1:13">
@@ -1900,10 +1909,10 @@
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>18</v>
@@ -1912,16 +1921,16 @@
         <v>19</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K9" s="5">
         <v>17765476062</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" ht="62" spans="1:13">
@@ -1941,28 +1950,28 @@
         <v>15</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" ht="82" spans="1:13">
@@ -1982,28 +1991,28 @@
         <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" ht="82" spans="1:13">
@@ -2023,10 +2032,10 @@
         <v>15</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>18</v>
@@ -2035,16 +2044,16 @@
         <v>19</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" ht="82" spans="1:13">
@@ -2064,10 +2073,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>18</v>
@@ -2076,16 +2085,16 @@
         <v>19</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" ht="123" spans="1:13">
@@ -2105,10 +2114,10 @@
         <v>15</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>18</v>
@@ -2117,16 +2126,16 @@
         <v>19</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K14" s="5">
         <v>15881979454</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" ht="82" spans="1:13">
@@ -2146,10 +2155,10 @@
         <v>15</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>18</v>
@@ -2158,16 +2167,16 @@
         <v>19</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" ht="143" spans="1:13">
@@ -2187,10 +2196,10 @@
         <v>15</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>18</v>
@@ -2199,16 +2208,16 @@
         <v>19</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K16" s="5">
         <v>18160066201</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" ht="82" spans="1:13">
@@ -2228,28 +2237,28 @@
         <v>15</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" ht="82" spans="1:13">
@@ -2263,16 +2272,16 @@
         <v>2.7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>18</v>
@@ -2281,16 +2290,16 @@
         <v>19</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" ht="62" spans="1:13">
@@ -2310,28 +2319,28 @@
         <v>15</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" ht="62" spans="1:13">
@@ -2351,28 +2360,28 @@
         <v>15</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" ht="82" spans="1:13">
@@ -2392,25 +2401,25 @@
         <v>15</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>22</v>
@@ -2433,25 +2442,25 @@
         <v>15</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>22</v>

</xml_diff>